<commit_message>
typos in microscopy file
</commit_message>
<xml_diff>
--- a/data/microscopy/microscopy.xlsx
+++ b/data/microscopy/microscopy.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CH-May" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="176">
   <si>
     <t xml:space="preserve">tube_id</t>
   </si>
@@ -492,9 +492,6 @@
   </si>
   <si>
     <t xml:space="preserve">CH205</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chironomidae_</t>
   </si>
   <si>
     <t xml:space="preserve">Hyphydrus_sp.</t>
@@ -664,23 +661,23 @@
   </sheetPr>
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G90" activeCellId="0" sqref="G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7908163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1020" min="8" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1021" min="1021" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1023" min="1022" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.4081632653061"/>
+    <col collapsed="false" hidden="false" max="1020" min="8" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1021" min="1021" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1023" min="1022" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="13.7704081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2833,24 +2830,24 @@
   </sheetPr>
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J71" activeCellId="0" sqref="J71"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.0714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="1020" min="9" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1021" min="1021" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1022" min="1022" style="0" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.6224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1020" min="9" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1021" min="1021" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1022" min="1022" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="13.7704081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3263,7 +3260,7 @@
         <v>41</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>157</v>
+        <v>41</v>
       </c>
       <c r="H16" s="0" t="n">
         <v>2</v>
@@ -3289,7 +3286,7 @@
         <v>20</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H17" s="0" t="n">
         <v>1</v>
@@ -3445,7 +3442,7 @@
         <v>93</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H23" s="0" t="n">
         <v>1</v>
@@ -3453,7 +3450,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B24" s="3" t="n">
         <v>43010</v>
@@ -3468,10 +3465,10 @@
         <v>40</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H24" s="0" t="n">
         <v>2</v>
@@ -3494,7 +3491,7 @@
         <v>32</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>34</v>
@@ -3531,7 +3528,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B27" s="3" t="n">
         <v>43010</v>
@@ -3557,7 +3554,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B28" s="3" t="n">
         <v>43010</v>
@@ -3583,7 +3580,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B29" s="3" t="n">
         <v>43010</v>
@@ -3609,7 +3606,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B30" s="3" t="n">
         <v>43010</v>
@@ -3635,7 +3632,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B31" s="3" t="n">
         <v>43010</v>
@@ -3754,10 +3751,10 @@
         <v>19</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H35" s="0" t="n">
         <v>1</v>
@@ -3817,7 +3814,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B38" s="3" t="n">
         <v>43010</v>
@@ -3913,7 +3910,7 @@
         <v>152</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H41" s="0" t="n">
         <v>2</v>
@@ -4014,7 +4011,7 @@
         <v>32</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G45" s="0" t="s">
         <v>34</v>
@@ -4118,10 +4115,10 @@
         <v>40</v>
       </c>
       <c r="F49" s="0" t="s">
+        <v>170</v>
+      </c>
+      <c r="G49" s="0" t="s">
         <v>171</v>
-      </c>
-      <c r="G49" s="0" t="s">
-        <v>172</v>
       </c>
       <c r="H49" s="0" t="n">
         <v>1</v>
@@ -4430,7 +4427,7 @@
         <v>32</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G61" s="0" t="s">
         <v>34</v>
@@ -4508,10 +4505,10 @@
         <v>151</v>
       </c>
       <c r="F64" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="G64" s="0" t="s">
         <v>173</v>
-      </c>
-      <c r="G64" s="0" t="s">
-        <v>174</v>
       </c>
       <c r="H64" s="0" t="n">
         <v>4</v>
@@ -4641,7 +4638,7 @@
         <v>93</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H69" s="0" t="n">
         <v>7</v>
@@ -4742,10 +4739,10 @@
         <v>40</v>
       </c>
       <c r="F73" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G73" s="0" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H73" s="0" t="n">
         <v>2</v>
@@ -4768,10 +4765,10 @@
         <v>40</v>
       </c>
       <c r="F74" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G74" s="0" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H74" s="0" t="n">
         <v>2</v>

</xml_diff>